<commit_message>
DDL y Esquema Actualizados para los Inserts
</commit_message>
<xml_diff>
--- a/SQL/Esquema SQL Excel.xlsx
+++ b/SQL/Esquema SQL Excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="88">
   <si>
     <t>servicio</t>
   </si>
@@ -266,21 +266,9 @@
     <t>matricula</t>
   </si>
   <si>
-    <t>Contacto</t>
-  </si>
-  <si>
     <t>id_contacto</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>facebook</t>
-  </si>
-  <si>
-    <t>instagram</t>
-  </si>
-  <si>
     <t>descuento</t>
   </si>
   <si>
@@ -294,6 +282,12 @@
   </si>
   <si>
     <t>legajo</t>
+  </si>
+  <si>
+    <t>e-mail</t>
+  </si>
+  <si>
+    <t>fecha_baja</t>
   </si>
 </sst>
 </file>
@@ -422,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -482,15 +476,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -498,7 +483,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -517,7 +502,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -529,12 +513,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -571,59 +555,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Conector recto de flecha 24"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="13249275" y="1571625"/>
-          <a:ext cx="66675" cy="1143001"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
@@ -918,8 +849,8 @@
         </a:xfrm>
         <a:prstGeom prst="arc">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 16200000"/>
-            <a:gd name="adj2" fmla="val 5636372"/>
+            <a:gd name="adj1" fmla="val 16353540"/>
+            <a:gd name="adj2" fmla="val 5402734"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1155,59 +1086,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="112" name="Conector recto de flecha 111"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14506575" y="2790825"/>
-          <a:ext cx="523875" cy="161925"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>476248</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -1270,13 +1148,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1378,26 +1256,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>285747</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Arco 46"/>
+        <xdr:cNvPr id="49" name="Arco 48"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="2362199" y="1428749"/>
-          <a:ext cx="504823" cy="1762125"/>
+          <a:off x="11172824" y="1228722"/>
+          <a:ext cx="257176" cy="1914527"/>
         </a:xfrm>
         <a:prstGeom prst="arc">
           <a:avLst>
@@ -1438,76 +1316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>66673</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>200021</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>133348</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Arco 48"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="11172824" y="1209673"/>
-          <a:ext cx="285747" cy="1590675"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 16200000"/>
-            <a:gd name="adj2" fmla="val 5309620"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="6D89FF"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114302</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1516,8 +1334,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3810000" y="1352550"/>
-          <a:ext cx="809625" cy="1047752"/>
+          <a:off x="3619500" y="1352550"/>
+          <a:ext cx="990600" cy="1228725"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1555,9 +1373,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1566,8 +1384,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3571875" y="495300"/>
-          <a:ext cx="923925" cy="638175"/>
+          <a:off x="3600450" y="495300"/>
+          <a:ext cx="885825" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1704,6 +1522,218 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Conector recto de flecha 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13211175" y="1543051"/>
+          <a:ext cx="0" cy="1523999"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Conector recto de flecha 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="13268325" y="3248025"/>
+          <a:ext cx="9526" cy="390526"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector recto de flecha 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13220700" y="4210050"/>
+          <a:ext cx="0" cy="390526"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Conector recto de flecha 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14382750" y="2790825"/>
+          <a:ext cx="523875" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1975,7 +2005,7 @@
   <dimension ref="B1:AR33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,10 +2026,10 @@
     <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.7109375" style="26" customWidth="1"/>
+    <col min="31" max="31" width="5.7109375" style="25" customWidth="1"/>
     <col min="32" max="32" width="72.42578125" customWidth="1"/>
     <col min="33" max="33" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19" bestFit="1" customWidth="1"/>
@@ -2015,46 +2045,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="27"/>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="26"/>
     </row>
     <row r="2" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="33" t="s">
         <v>50</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="P2" s="26"/>
-      <c r="AG2" s="27"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="27"/>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="27"/>
-      <c r="AN2" s="27"/>
-      <c r="AO2" s="27"/>
-      <c r="AP2" s="27"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="27"/>
+      <c r="I2" s="23"/>
+      <c r="P2" s="25"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="26"/>
     </row>
     <row r="3" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>51</v>
       </c>
       <c r="D3" t="s">
@@ -2066,17 +2096,17 @@
       <c r="G3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="24"/>
+      <c r="H3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="23"/>
       <c r="K3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="26"/>
+      <c r="P3" s="25"/>
       <c r="S3" s="8" t="s">
         <v>19</v>
       </c>
@@ -2086,21 +2116,21 @@
       <c r="Z3" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AD3" s="28" t="s">
+      <c r="AD3" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="AG3" s="27"/>
-      <c r="AH3" s="32"/>
-      <c r="AI3" s="27"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="27"/>
-      <c r="AL3" s="27"/>
-      <c r="AM3" s="27"/>
-      <c r="AN3" s="27"/>
-      <c r="AO3" s="27"/>
-      <c r="AP3" s="27"/>
-      <c r="AQ3" s="33"/>
-      <c r="AR3" s="27"/>
+      <c r="AG3" s="26"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="26"/>
+      <c r="AJ3" s="26"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="26"/>
+      <c r="AM3" s="26"/>
+      <c r="AN3" s="26"/>
+      <c r="AO3" s="26"/>
+      <c r="AP3" s="26"/>
+      <c r="AQ3" s="31"/>
+      <c r="AR3" s="26"/>
     </row>
     <row r="4" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
@@ -2112,10 +2142,10 @@
       <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="24"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="2" t="s">
         <v>35</v>
       </c>
@@ -2131,7 +2161,7 @@
       <c r="O4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="26" t="s">
         <v>57</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -2140,16 +2170,16 @@
       <c r="S4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>57</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="W4" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="W4" s="24" t="s">
         <v>57</v>
       </c>
       <c r="Y4" s="2" t="s">
@@ -2158,7 +2188,7 @@
       <c r="Z4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="27" t="s">
+      <c r="AA4" s="26" t="s">
         <v>57</v>
       </c>
       <c r="AC4" s="2" t="s">
@@ -2167,28 +2197,28 @@
       <c r="AD4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="AE4" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG4" s="27"/>
-      <c r="AH4" s="32"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="27"/>
-      <c r="AM4" s="27"/>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="33"/>
-      <c r="AR4" s="27"/>
+      <c r="AE4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="26"/>
+      <c r="AJ4" s="26"/>
+      <c r="AK4" s="26"/>
+      <c r="AL4" s="26"/>
+      <c r="AM4" s="26"/>
+      <c r="AN4" s="26"/>
+      <c r="AO4" s="26"/>
+      <c r="AP4" s="26"/>
+      <c r="AQ4" s="31"/>
+      <c r="AR4" s="26"/>
     </row>
     <row r="5" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
@@ -2199,7 +2229,7 @@
       <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="1" t="s">
         <v>36</v>
       </c>
@@ -2212,52 +2242,49 @@
       <c r="O5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="27" t="s">
+      <c r="P5" s="26" t="s">
         <v>59</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="24" t="s">
+      <c r="T5" s="23" t="s">
         <v>58</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W5" s="24" t="s">
+      <c r="W5" s="23" t="s">
         <v>58</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AA5" s="27" t="s">
+      <c r="AA5" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AD5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AE5" s="27" t="s">
+      <c r="AE5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="32"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="27"/>
-      <c r="AM5" s="27"/>
-      <c r="AN5" s="27"/>
-      <c r="AO5" s="27"/>
-      <c r="AP5" s="27"/>
-      <c r="AQ5" s="33"/>
-      <c r="AR5" s="27"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="26"/>
+      <c r="AK5" s="26"/>
+      <c r="AL5" s="26"/>
+      <c r="AM5" s="26"/>
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="26"/>
+      <c r="AP5" s="26"/>
+      <c r="AQ5" s="31"/>
+      <c r="AR5" s="26"/>
     </row>
     <row r="6" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>81</v>
+      <c r="C6" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -2271,7 +2298,7 @@
       <c r="H6" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="24"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2287,7 +2314,7 @@
       <c r="O6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="26" t="s">
         <v>57</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -2299,25 +2326,25 @@
       <c r="Z6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AA6" s="27" t="s">
+      <c r="AA6" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="AG6" s="27"/>
-      <c r="AH6" s="32"/>
-      <c r="AI6" s="27"/>
-      <c r="AJ6" s="27"/>
-      <c r="AK6" s="27"/>
-      <c r="AL6" s="27"/>
-      <c r="AM6" s="27"/>
-      <c r="AN6" s="27"/>
-      <c r="AO6" s="27"/>
-      <c r="AP6" s="27"/>
-      <c r="AQ6" s="33"/>
-      <c r="AR6" s="27"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="30"/>
+      <c r="AI6" s="26"/>
+      <c r="AJ6" s="26"/>
+      <c r="AK6" s="26"/>
+      <c r="AL6" s="26"/>
+      <c r="AM6" s="26"/>
+      <c r="AN6" s="26"/>
+      <c r="AO6" s="26"/>
+      <c r="AP6" s="26"/>
+      <c r="AQ6" s="31"/>
+      <c r="AR6" s="26"/>
     </row>
     <row r="7" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>49</v>
+      <c r="C7" s="17" t="s">
+        <v>86</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
@@ -2331,7 +2358,7 @@
       <c r="H7" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2347,7 +2374,7 @@
       <c r="O7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="27" t="s">
+      <c r="P7" s="26" t="s">
         <v>57</v>
       </c>
       <c r="S7" s="8" t="s">
@@ -2368,43 +2395,40 @@
       <c r="Z7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AA7" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG7" s="27"/>
-      <c r="AH7" s="32"/>
-      <c r="AI7" s="27"/>
-      <c r="AJ7" s="27"/>
-      <c r="AK7" s="27"/>
-      <c r="AL7" s="27"/>
-      <c r="AM7" s="27"/>
-      <c r="AN7" s="27"/>
-      <c r="AO7" s="27"/>
-      <c r="AP7" s="27"/>
-      <c r="AQ7" s="34"/>
-      <c r="AR7" s="27"/>
+      <c r="AA7" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG7" s="26"/>
+      <c r="AH7" s="30"/>
+      <c r="AI7" s="26"/>
+      <c r="AJ7" s="26"/>
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="26"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="26"/>
+      <c r="AQ7" s="32"/>
+      <c r="AR7" s="26"/>
     </row>
     <row r="8" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>81</v>
+        <v>58</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="H8" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="I8" s="23"/>
       <c r="K8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="23" t="s">
         <v>60</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -2413,7 +2437,7 @@
       <c r="O8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="26" t="s">
+      <c r="P8" s="25" t="s">
         <v>57</v>
       </c>
       <c r="R8" s="2" t="s">
@@ -2440,43 +2464,40 @@
       <c r="Z8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="32"/>
-      <c r="AI8" s="27"/>
-      <c r="AJ8" s="27"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="27"/>
-      <c r="AM8" s="27"/>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="27"/>
-      <c r="AR8" s="27"/>
+      <c r="AA8" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="30"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
+      <c r="AM8" s="26"/>
+      <c r="AN8" s="26"/>
+      <c r="AO8" s="26"/>
+      <c r="AP8" s="26"/>
+      <c r="AQ8" s="26"/>
+      <c r="AR8" s="26"/>
     </row>
     <row r="9" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>12</v>
+      <c r="C9" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>57</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="24"/>
-      <c r="K9" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="K9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="23" t="s">
         <v>57</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -2485,55 +2506,61 @@
       <c r="O9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P9" s="26" t="s">
+      <c r="P9" s="25" t="s">
         <v>57</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="T9" s="24" t="s">
+      <c r="T9" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="U9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>81</v>
+      <c r="V9" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="W9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Z9" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AA9" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="32"/>
-      <c r="AI9" s="27"/>
-      <c r="AJ9" s="27"/>
-      <c r="AK9" s="27"/>
-      <c r="AL9" s="27"/>
-      <c r="AM9" s="27"/>
-      <c r="AN9" s="27"/>
-      <c r="AO9" s="27"/>
-      <c r="AP9" s="27"/>
-      <c r="AQ9" s="27"/>
-      <c r="AR9" s="27"/>
+      <c r="AA9" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="26"/>
+      <c r="AO9" s="26"/>
+      <c r="AP9" s="26"/>
+      <c r="AQ9" s="26"/>
+      <c r="AR9" s="26"/>
     </row>
     <row r="10" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="G10" s="4" t="s">
-        <v>13</v>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>79</v>
       </c>
       <c r="H10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" s="24" t="s">
+      <c r="K10" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="23" t="s">
         <v>57</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -2542,90 +2569,80 @@
       <c r="O10" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="23" t="s">
         <v>57</v>
       </c>
       <c r="V10" s="17" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="W10" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z10" s="6" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="Z10" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="AA10" t="s">
         <v>57</v>
       </c>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="27"/>
-      <c r="AL10" s="27"/>
-      <c r="AM10" s="27"/>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="27"/>
-      <c r="AR10" s="27"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="26"/>
+      <c r="AM10" s="26"/>
+      <c r="AN10" s="26"/>
+      <c r="AO10" s="26"/>
+      <c r="AP10" s="26"/>
+      <c r="AQ10" s="26"/>
+      <c r="AR10" s="26"/>
     </row>
     <row r="11" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C11" s="21" t="s">
-        <v>52</v>
+      <c r="G11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="V11" s="17" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="W11" t="s">
         <v>59</v>
       </c>
-      <c r="Z11" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA11" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="27"/>
-      <c r="AJ11" s="27"/>
-      <c r="AK11" s="27"/>
-      <c r="AL11" s="27"/>
-      <c r="AM11" s="27"/>
-      <c r="AN11" s="27"/>
-      <c r="AO11" s="27"/>
-      <c r="AP11" s="27"/>
-      <c r="AQ11" s="27"/>
-      <c r="AR11" s="27"/>
+      <c r="Z11" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG11" s="26"/>
+      <c r="AH11" s="26"/>
+      <c r="AI11" s="26"/>
+      <c r="AJ11" s="26"/>
+      <c r="AK11" s="26"/>
+      <c r="AL11" s="26"/>
+      <c r="AM11" s="26"/>
+      <c r="AN11" s="26"/>
+      <c r="AO11" s="26"/>
+      <c r="AP11" s="26"/>
+      <c r="AQ11" s="26"/>
+      <c r="AR11" s="26"/>
     </row>
     <row r="12" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="26"/>
+      <c r="C12" s="20" t="s">
+        <v>52</v>
+      </c>
       <c r="K12" s="14" t="s">
         <v>39</v>
       </c>
       <c r="O12" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="P12" s="26"/>
+      <c r="P12" s="25"/>
       <c r="R12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2635,41 +2652,45 @@
       <c r="T12" t="s">
         <v>57</v>
       </c>
-      <c r="V12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="W12" s="24" t="s">
+      <c r="V12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="W12" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="27"/>
-      <c r="AI12" s="27"/>
-      <c r="AJ12" s="27"/>
-      <c r="AK12" s="27"/>
-      <c r="AL12" s="27"/>
-      <c r="AM12" s="27"/>
-      <c r="AN12" s="27"/>
-      <c r="AO12" s="27"/>
-      <c r="AP12" s="27"/>
-      <c r="AQ12" s="27"/>
-      <c r="AR12" s="27"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="26"/>
+      <c r="AK12" s="26"/>
+      <c r="AL12" s="26"/>
+      <c r="AM12" s="26"/>
+      <c r="AN12" s="26"/>
+      <c r="AO12" s="26"/>
+      <c r="AP12" s="26"/>
+      <c r="AQ12" s="26"/>
+      <c r="AR12" s="26"/>
     </row>
     <row r="13" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C13" s="3" t="s">
-        <v>1</v>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>57</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="25"/>
       <c r="J13" s="2" t="s">
         <v>35</v>
       </c>
@@ -2685,7 +2706,7 @@
       <c r="O13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="P13" s="26" t="s">
+      <c r="P13" s="25" t="s">
         <v>57</v>
       </c>
       <c r="R13" s="1" t="s">
@@ -2697,34 +2718,40 @@
       <c r="T13" t="s">
         <v>57</v>
       </c>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="27"/>
-      <c r="AI13" s="27"/>
-      <c r="AJ13" s="27"/>
-      <c r="AK13" s="27"/>
-      <c r="AL13" s="27"/>
-      <c r="AM13" s="27"/>
-      <c r="AN13" s="27"/>
-      <c r="AO13" s="27"/>
-      <c r="AP13" s="27"/>
-      <c r="AQ13" s="27"/>
-      <c r="AR13" s="27"/>
+      <c r="V13" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="W13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+      <c r="AL13" s="26"/>
+      <c r="AM13" s="26"/>
+      <c r="AN13" s="26"/>
+      <c r="AO13" s="26"/>
+      <c r="AP13" s="26"/>
+      <c r="AQ13" s="26"/>
+      <c r="AR13" s="26"/>
     </row>
     <row r="14" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>51</v>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>10</v>
@@ -2735,7 +2762,7 @@
       <c r="O14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="27" t="s">
+      <c r="P14" s="26" t="s">
         <v>58</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -2747,187 +2774,158 @@
       <c r="T14" t="s">
         <v>57</v>
       </c>
-      <c r="V14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="27"/>
-      <c r="AI14" s="27"/>
-      <c r="AJ14" s="27"/>
-      <c r="AK14" s="33"/>
-      <c r="AL14" s="27"/>
-      <c r="AM14" s="27"/>
-      <c r="AN14" s="27"/>
-      <c r="AO14" s="27"/>
-      <c r="AP14" s="27"/>
-      <c r="AQ14" s="27"/>
-      <c r="AR14" s="27"/>
+      <c r="V14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="W14" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="31"/>
+      <c r="AL14" s="26"/>
+      <c r="AM14" s="26"/>
+      <c r="AN14" s="26"/>
+      <c r="AO14" s="26"/>
+      <c r="AP14" s="26"/>
+      <c r="AQ14" s="26"/>
+      <c r="AR14" s="26"/>
     </row>
     <row r="15" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
         <v>57</v>
       </c>
+      <c r="G15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>58</v>
+      </c>
       <c r="O15" s="13"/>
-      <c r="P15" s="26"/>
+      <c r="P15" s="25"/>
       <c r="S15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="T15" t="s">
         <v>57</v>
       </c>
-      <c r="U15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V15" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="W15" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA15" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="27"/>
-      <c r="AI15" s="27"/>
-      <c r="AJ15" s="27"/>
-      <c r="AK15" s="27"/>
-      <c r="AL15" s="27"/>
-      <c r="AM15" s="27"/>
-      <c r="AN15" s="27"/>
-      <c r="AO15" s="27"/>
-      <c r="AP15" s="27"/>
-      <c r="AQ15" s="27"/>
-      <c r="AR15" s="27"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
+      <c r="AI15" s="26"/>
+      <c r="AJ15" s="26"/>
+      <c r="AK15" s="26"/>
+      <c r="AL15" s="26"/>
+      <c r="AM15" s="26"/>
+      <c r="AN15" s="26"/>
+      <c r="AO15" s="26"/>
+      <c r="AP15" s="26"/>
+      <c r="AQ15" s="26"/>
+      <c r="AR15" s="26"/>
     </row>
     <row r="16" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>22</v>
+      <c r="C16" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="P16" s="25"/>
       <c r="S16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="T16" s="24" t="s">
+      <c r="T16" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="V16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="W16" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA16" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD16" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE16" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
-      <c r="AI16" s="27"/>
-      <c r="AJ16" s="27"/>
-      <c r="AK16" s="27"/>
-      <c r="AL16" s="27"/>
-      <c r="AM16" s="27"/>
-      <c r="AN16" s="27"/>
-      <c r="AO16" s="27"/>
-      <c r="AP16" s="27"/>
-      <c r="AQ16" s="27"/>
-      <c r="AR16" s="27"/>
+      <c r="V16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG16" s="26"/>
+      <c r="AH16" s="26"/>
+      <c r="AI16" s="26"/>
+      <c r="AJ16" s="26"/>
+      <c r="AK16" s="26"/>
+      <c r="AL16" s="26"/>
+      <c r="AM16" s="26"/>
+      <c r="AN16" s="26"/>
+      <c r="AO16" s="26"/>
+      <c r="AP16" s="26"/>
+      <c r="AQ16" s="26"/>
+      <c r="AR16" s="26"/>
     </row>
     <row r="17" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="F17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H17" s="27" t="s">
-        <v>57</v>
-      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="26"/>
       <c r="K17" s="14" t="s">
         <v>37</v>
       </c>
       <c r="O17" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="P17" s="26"/>
+      <c r="P17" s="25"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="24"/>
-      <c r="Y17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA17" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE17" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="27"/>
-      <c r="AI17" s="27"/>
-      <c r="AJ17" s="27"/>
-      <c r="AK17" s="27"/>
-      <c r="AL17" s="27"/>
-      <c r="AM17" s="27"/>
-      <c r="AN17" s="27"/>
-      <c r="AO17" s="27"/>
-      <c r="AP17" s="27"/>
-      <c r="AQ17" s="27"/>
-      <c r="AR17" s="27"/>
+      <c r="S17" s="29"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="V17" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="W17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA17" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD17" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG17" s="26"/>
+      <c r="AH17" s="26"/>
+      <c r="AI17" s="26"/>
+      <c r="AJ17" s="26"/>
+      <c r="AK17" s="26"/>
+      <c r="AL17" s="26"/>
+      <c r="AM17" s="26"/>
+      <c r="AN17" s="26"/>
+      <c r="AO17" s="26"/>
+      <c r="AP17" s="26"/>
+      <c r="AQ17" s="26"/>
+      <c r="AR17" s="26"/>
     </row>
     <row r="18" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="G18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>58</v>
-      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="26"/>
       <c r="J18" s="2" t="s">
         <v>35</v>
       </c>
@@ -2940,41 +2938,49 @@
       <c r="N18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O18" s="22" t="s">
+      <c r="O18" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="P18" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE18" s="27" t="s">
+      <c r="P18" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="W18" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="27"/>
-      <c r="AI18" s="27"/>
-      <c r="AJ18" s="27"/>
-      <c r="AK18" s="27"/>
-      <c r="AL18" s="27"/>
-      <c r="AM18" s="27"/>
-      <c r="AN18" s="27"/>
-      <c r="AO18" s="27"/>
-      <c r="AP18" s="27"/>
-      <c r="AQ18" s="27"/>
-      <c r="AR18" s="27"/>
+      <c r="Z18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA18" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD18" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE18" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG18" s="26"/>
+      <c r="AH18" s="26"/>
+      <c r="AI18" s="26"/>
+      <c r="AJ18" s="26"/>
+      <c r="AK18" s="26"/>
+      <c r="AL18" s="26"/>
+      <c r="AM18" s="26"/>
+      <c r="AN18" s="26"/>
+      <c r="AO18" s="26"/>
+      <c r="AP18" s="26"/>
+      <c r="AQ18" s="26"/>
+      <c r="AR18" s="26"/>
     </row>
     <row r="19" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C19" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>57</v>
-      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="26"/>
       <c r="K19" s="3" t="s">
         <v>44</v>
       </c>
@@ -2984,50 +2990,43 @@
       <c r="O19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P19" s="27" t="s">
+      <c r="P19" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Z19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC19" s="1" t="s">
+      <c r="Y19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE19" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG19" s="27"/>
-      <c r="AH19" s="27"/>
-      <c r="AI19" s="27"/>
-      <c r="AJ19" s="27"/>
-      <c r="AK19" s="27"/>
-      <c r="AL19" s="27"/>
-      <c r="AM19" s="27"/>
-      <c r="AN19" s="27"/>
-      <c r="AO19" s="27"/>
-      <c r="AP19" s="27"/>
-      <c r="AQ19" s="27"/>
-      <c r="AR19" s="27"/>
+      <c r="Z19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG19" s="26"/>
+      <c r="AH19" s="26"/>
+      <c r="AI19" s="26"/>
+      <c r="AJ19" s="26"/>
+      <c r="AK19" s="26"/>
+      <c r="AL19" s="26"/>
+      <c r="AM19" s="26"/>
+      <c r="AN19" s="26"/>
+      <c r="AO19" s="26"/>
+      <c r="AP19" s="26"/>
+      <c r="AQ19" s="26"/>
+      <c r="AR19" s="26"/>
     </row>
     <row r="20" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="27" t="s">
-        <v>58</v>
-      </c>
+      <c r="C20" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="26"/>
       <c r="J20" s="1" t="s">
         <v>36</v>
       </c>
@@ -3040,56 +3039,40 @@
       <c r="O20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P20" s="27" t="s">
+      <c r="P20" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Y20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z20" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA20" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD20" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG20" s="27"/>
-      <c r="AH20" s="27"/>
-      <c r="AI20" s="27"/>
-      <c r="AJ20" s="27"/>
-      <c r="AK20" s="27"/>
-      <c r="AL20" s="27"/>
-      <c r="AM20" s="27"/>
-      <c r="AN20" s="27"/>
-      <c r="AO20" s="27"/>
-      <c r="AP20" s="27"/>
-      <c r="AQ20" s="27"/>
-      <c r="AR20" s="27"/>
+      <c r="AD20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="26"/>
+      <c r="AI20" s="26"/>
+      <c r="AJ20" s="26"/>
+      <c r="AK20" s="26"/>
+      <c r="AL20" s="26"/>
+      <c r="AM20" s="26"/>
+      <c r="AN20" s="26"/>
+      <c r="AO20" s="26"/>
+      <c r="AP20" s="26"/>
+      <c r="AQ20" s="26"/>
+      <c r="AR20" s="26"/>
     </row>
     <row r="21" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>53</v>
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>58</v>
-      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="26"/>
       <c r="J21" s="1" t="s">
         <v>36</v>
       </c>
@@ -3102,36 +3085,37 @@
       <c r="O21" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="27" t="s">
+      <c r="P21" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="Z21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA21" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD21" s="30"/>
-      <c r="AE21" s="27"/>
-      <c r="AG21" s="27"/>
-      <c r="AH21" s="27"/>
-      <c r="AI21" s="27"/>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="27"/>
-      <c r="AL21" s="27"/>
-      <c r="AM21" s="27"/>
-      <c r="AN21" s="27"/>
-      <c r="AO21" s="27"/>
-      <c r="AP21" s="27"/>
-      <c r="AQ21" s="27"/>
-      <c r="AR21" s="27"/>
+      <c r="Z21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE21" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG21" s="26"/>
+      <c r="AH21" s="26"/>
+      <c r="AI21" s="26"/>
+      <c r="AJ21" s="26"/>
+      <c r="AK21" s="26"/>
+      <c r="AL21" s="26"/>
+      <c r="AM21" s="26"/>
+      <c r="AN21" s="26"/>
+      <c r="AO21" s="26"/>
+      <c r="AP21" s="26"/>
+      <c r="AQ21" s="26"/>
+      <c r="AR21" s="26"/>
     </row>
     <row r="22" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
         <v>57</v>
@@ -3142,34 +3126,43 @@
       <c r="O22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P22" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z22" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA22" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG22" s="27"/>
-      <c r="AH22" s="27"/>
-      <c r="AI22" s="27"/>
-      <c r="AJ22" s="27"/>
-      <c r="AK22" s="27"/>
-      <c r="AL22" s="27"/>
-      <c r="AM22" s="27"/>
-      <c r="AN22" s="27"/>
-      <c r="AO22" s="27"/>
-      <c r="AP22" s="27"/>
-      <c r="AQ22" s="27"/>
-      <c r="AR22" s="27"/>
+      <c r="P22" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA22" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD22" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG22" s="26"/>
+      <c r="AH22" s="26"/>
+      <c r="AI22" s="26"/>
+      <c r="AJ22" s="26"/>
+      <c r="AK22" s="26"/>
+      <c r="AL22" s="26"/>
+      <c r="AM22" s="26"/>
+      <c r="AN22" s="26"/>
+      <c r="AO22" s="26"/>
+      <c r="AP22" s="26"/>
+      <c r="AQ22" s="26"/>
+      <c r="AR22" s="26"/>
     </row>
     <row r="23" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
-        <v>4</v>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>57</v>
@@ -3180,28 +3173,43 @@
       <c r="O23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P23" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG23" s="27"/>
-      <c r="AH23" s="27"/>
-      <c r="AI23" s="27"/>
-      <c r="AJ23" s="27"/>
-      <c r="AK23" s="27"/>
-      <c r="AL23" s="27"/>
-      <c r="AM23" s="27"/>
-      <c r="AN23" s="27"/>
-      <c r="AO23" s="27"/>
-      <c r="AP23" s="27"/>
-      <c r="AQ23" s="27"/>
-      <c r="AR23" s="27"/>
+      <c r="P23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA23" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG23" s="26"/>
+      <c r="AH23" s="26"/>
+      <c r="AI23" s="26"/>
+      <c r="AJ23" s="26"/>
+      <c r="AK23" s="26"/>
+      <c r="AL23" s="26"/>
+      <c r="AM23" s="26"/>
+      <c r="AN23" s="26"/>
+      <c r="AO23" s="26"/>
+      <c r="AP23" s="26"/>
+      <c r="AQ23" s="26"/>
+      <c r="AR23" s="26"/>
     </row>
     <row r="24" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
-        <v>2</v>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>7</v>
@@ -3212,26 +3220,47 @@
       <c r="O24" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="P24" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z24" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG24" s="27"/>
-      <c r="AH24" s="27"/>
-      <c r="AI24" s="27"/>
-      <c r="AJ24" s="27"/>
-      <c r="AK24" s="27"/>
-      <c r="AL24" s="27"/>
-      <c r="AM24" s="27"/>
-      <c r="AN24" s="27"/>
-      <c r="AO24" s="27"/>
-      <c r="AP24" s="27"/>
-      <c r="AQ24" s="27"/>
-      <c r="AR24" s="27"/>
+      <c r="P24" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z24" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA24" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG24" s="26"/>
+      <c r="AH24" s="26"/>
+      <c r="AI24" s="26"/>
+      <c r="AJ24" s="26"/>
+      <c r="AK24" s="26"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="26"/>
+      <c r="AN24" s="26"/>
+      <c r="AO24" s="26"/>
+      <c r="AP24" s="26"/>
+      <c r="AQ24" s="26"/>
+      <c r="AR24" s="26"/>
     </row>
     <row r="25" spans="2:44" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
       <c r="J25" s="2" t="s">
         <v>35</v>
       </c>
@@ -3247,178 +3276,181 @@
       <c r="O25" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P25" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA25" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG25" s="27"/>
-      <c r="AH25" s="27"/>
-      <c r="AI25" s="27"/>
-      <c r="AJ25" s="27"/>
-      <c r="AK25" s="27"/>
-      <c r="AL25" s="27"/>
-      <c r="AM25" s="27"/>
-      <c r="AN25" s="27"/>
-      <c r="AO25" s="27"/>
-      <c r="AP25" s="27"/>
-      <c r="AQ25" s="27"/>
-      <c r="AR25" s="27"/>
+      <c r="P25" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG25" s="26"/>
+      <c r="AH25" s="26"/>
+      <c r="AI25" s="26"/>
+      <c r="AJ25" s="26"/>
+      <c r="AK25" s="26"/>
+      <c r="AL25" s="26"/>
+      <c r="AM25" s="26"/>
+      <c r="AN25" s="26"/>
+      <c r="AO25" s="26"/>
+      <c r="AP25" s="26"/>
+      <c r="AQ25" s="26"/>
+      <c r="AR25" s="26"/>
     </row>
     <row r="26" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C26" s="21" t="s">
-        <v>88</v>
-      </c>
       <c r="K26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L26" t="s">
         <v>58</v>
       </c>
-      <c r="O26" s="23" t="s">
+      <c r="O26" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="P26" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA26" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG26" s="27"/>
-      <c r="AH26" s="27"/>
-      <c r="AI26" s="27"/>
-      <c r="AJ26" s="27"/>
-      <c r="AK26" s="27"/>
-      <c r="AL26" s="27"/>
-      <c r="AM26" s="27"/>
-      <c r="AN26" s="27"/>
-      <c r="AO26" s="27"/>
-      <c r="AP26" s="27"/>
-      <c r="AQ26" s="27"/>
-      <c r="AR26" s="27"/>
+      <c r="P26" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG26" s="26"/>
+      <c r="AH26" s="26"/>
+      <c r="AI26" s="26"/>
+      <c r="AJ26" s="26"/>
+      <c r="AK26" s="26"/>
+      <c r="AL26" s="26"/>
+      <c r="AM26" s="26"/>
+      <c r="AN26" s="26"/>
+      <c r="AO26" s="26"/>
+      <c r="AP26" s="26"/>
+      <c r="AQ26" s="26"/>
+      <c r="AR26" s="26"/>
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG27" s="27"/>
-      <c r="AH27" s="27"/>
-      <c r="AI27" s="27"/>
-      <c r="AJ27" s="27"/>
-      <c r="AK27" s="27"/>
-      <c r="AL27" s="27"/>
-      <c r="AM27" s="27"/>
-      <c r="AN27" s="27"/>
-      <c r="AO27" s="27"/>
-      <c r="AP27" s="27"/>
-      <c r="AQ27" s="27"/>
-      <c r="AR27" s="27"/>
+      <c r="Z27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA27" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG27" s="26"/>
+      <c r="AH27" s="26"/>
+      <c r="AI27" s="26"/>
+      <c r="AJ27" s="26"/>
+      <c r="AK27" s="26"/>
+      <c r="AL27" s="26"/>
+      <c r="AM27" s="26"/>
+      <c r="AN27" s="26"/>
+      <c r="AO27" s="26"/>
+      <c r="AP27" s="26"/>
+      <c r="AQ27" s="26"/>
+      <c r="AR27" s="26"/>
     </row>
     <row r="28" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
-        <v>3</v>
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>83</v>
       </c>
       <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA28" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="AG28" s="27"/>
-      <c r="AH28" s="27"/>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="27"/>
-      <c r="AK28" s="27"/>
-      <c r="AL28" s="27"/>
-      <c r="AM28" s="27"/>
-      <c r="AN28" s="27"/>
-      <c r="AO28" s="27"/>
-      <c r="AP28" s="27"/>
-      <c r="AQ28" s="27"/>
-      <c r="AR28" s="27"/>
+      <c r="AG28" s="26"/>
+      <c r="AH28" s="26"/>
+      <c r="AI28" s="26"/>
+      <c r="AJ28" s="26"/>
+      <c r="AK28" s="26"/>
+      <c r="AL28" s="26"/>
+      <c r="AM28" s="26"/>
+      <c r="AN28" s="26"/>
+      <c r="AO28" s="26"/>
+      <c r="AP28" s="26"/>
+      <c r="AQ28" s="26"/>
+      <c r="AR28" s="26"/>
     </row>
     <row r="29" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="27"/>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="27"/>
-      <c r="AK29" s="27"/>
-      <c r="AL29" s="27"/>
-      <c r="AM29" s="27"/>
-      <c r="AN29" s="27"/>
-      <c r="AO29" s="27"/>
-      <c r="AP29" s="27"/>
-      <c r="AQ29" s="27"/>
-      <c r="AR29" s="27"/>
+      <c r="C29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG29" s="26"/>
+      <c r="AH29" s="26"/>
+      <c r="AI29" s="26"/>
+      <c r="AJ29" s="26"/>
+      <c r="AK29" s="26"/>
+      <c r="AL29" s="26"/>
+      <c r="AM29" s="26"/>
+      <c r="AN29" s="26"/>
+      <c r="AO29" s="26"/>
+      <c r="AP29" s="26"/>
+      <c r="AQ29" s="26"/>
+      <c r="AR29" s="26"/>
     </row>
     <row r="30" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="AG30" s="27"/>
-      <c r="AH30" s="27"/>
-      <c r="AI30" s="27"/>
-      <c r="AJ30" s="27"/>
-      <c r="AK30" s="27"/>
-      <c r="AL30" s="27"/>
-      <c r="AM30" s="27"/>
-      <c r="AN30" s="27"/>
-      <c r="AO30" s="27"/>
-      <c r="AP30" s="27"/>
-      <c r="AQ30" s="27"/>
-      <c r="AR30" s="27"/>
+      <c r="AG30" s="26"/>
+      <c r="AH30" s="26"/>
+      <c r="AI30" s="26"/>
+      <c r="AJ30" s="26"/>
+      <c r="AK30" s="26"/>
+      <c r="AL30" s="26"/>
+      <c r="AM30" s="26"/>
+      <c r="AN30" s="26"/>
+      <c r="AO30" s="26"/>
+      <c r="AP30" s="26"/>
+      <c r="AQ30" s="26"/>
+      <c r="AR30" s="26"/>
     </row>
     <row r="31" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="AG31" s="27"/>
-      <c r="AH31" s="27"/>
-      <c r="AI31" s="27"/>
-      <c r="AJ31" s="27"/>
-      <c r="AK31" s="27"/>
-      <c r="AL31" s="27"/>
-      <c r="AM31" s="27"/>
-      <c r="AN31" s="27"/>
-      <c r="AO31" s="27"/>
-      <c r="AP31" s="27"/>
-      <c r="AQ31" s="27"/>
-      <c r="AR31" s="27"/>
+      <c r="AG31" s="26"/>
+      <c r="AH31" s="26"/>
+      <c r="AI31" s="26"/>
+      <c r="AJ31" s="26"/>
+      <c r="AK31" s="26"/>
+      <c r="AL31" s="26"/>
+      <c r="AM31" s="26"/>
+      <c r="AN31" s="26"/>
+      <c r="AO31" s="26"/>
+      <c r="AP31" s="26"/>
+      <c r="AQ31" s="26"/>
+      <c r="AR31" s="26"/>
     </row>
     <row r="32" spans="2:44" x14ac:dyDescent="0.25">
-      <c r="AG32" s="27"/>
-      <c r="AH32" s="27"/>
-      <c r="AI32" s="27"/>
-      <c r="AJ32" s="27"/>
-      <c r="AK32" s="27"/>
-      <c r="AL32" s="27"/>
-      <c r="AM32" s="27"/>
-      <c r="AN32" s="27"/>
-      <c r="AO32" s="27"/>
-      <c r="AP32" s="27"/>
-      <c r="AQ32" s="27"/>
-      <c r="AR32" s="27"/>
+      <c r="AG32" s="26"/>
+      <c r="AH32" s="26"/>
+      <c r="AI32" s="26"/>
+      <c r="AJ32" s="26"/>
+      <c r="AK32" s="26"/>
+      <c r="AL32" s="26"/>
+      <c r="AM32" s="26"/>
+      <c r="AN32" s="26"/>
+      <c r="AO32" s="26"/>
+      <c r="AP32" s="26"/>
+      <c r="AQ32" s="26"/>
+      <c r="AR32" s="26"/>
     </row>
     <row r="33" spans="33:44" x14ac:dyDescent="0.25">
-      <c r="AG33" s="27"/>
-      <c r="AH33" s="27"/>
-      <c r="AI33" s="27"/>
-      <c r="AJ33" s="27"/>
-      <c r="AK33" s="27"/>
-      <c r="AL33" s="27"/>
-      <c r="AM33" s="27"/>
-      <c r="AN33" s="27"/>
-      <c r="AO33" s="27"/>
-      <c r="AP33" s="27"/>
-      <c r="AQ33" s="27"/>
-      <c r="AR33" s="27"/>
+      <c r="AG33" s="26"/>
+      <c r="AH33" s="26"/>
+      <c r="AI33" s="26"/>
+      <c r="AJ33" s="26"/>
+      <c r="AK33" s="26"/>
+      <c r="AL33" s="26"/>
+      <c r="AM33" s="26"/>
+      <c r="AN33" s="26"/>
+      <c r="AO33" s="26"/>
+      <c r="AP33" s="26"/>
+      <c r="AQ33" s="26"/>
+      <c r="AR33" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Inserts de la BD, y Estructura actualizada
</commit_message>
<xml_diff>
--- a/SQL/Esquema SQL Excel.xlsx
+++ b/SQL/Esquema SQL Excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="85">
   <si>
     <t>servicio</t>
   </si>
@@ -137,154 +137,148 @@
     <t>(FK)</t>
   </si>
   <si>
+    <t>Tipos Productos</t>
+  </si>
+  <si>
+    <t>id_producto</t>
+  </si>
+  <si>
+    <t>id_caracteristica</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>Sedes</t>
+  </si>
+  <si>
+    <t>Puestos</t>
+  </si>
+  <si>
+    <t>puesto</t>
+  </si>
+  <si>
+    <t>id_sede</t>
+  </si>
+  <si>
+    <t>calle</t>
+  </si>
+  <si>
+    <t>Proveedores</t>
+  </si>
+  <si>
+    <t>id_proveedor</t>
+  </si>
+  <si>
+    <t>Pedidos</t>
+  </si>
+  <si>
+    <t>id_pedido</t>
+  </si>
+  <si>
+    <t>Detalle Pedido</t>
+  </si>
+  <si>
+    <t>id_det_ped</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>precio compra</t>
+  </si>
+  <si>
+    <t>id_puesto</t>
+  </si>
+  <si>
+    <t>Paises</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Medicos</t>
+  </si>
+  <si>
+    <t>Empleados</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>sueldo</t>
+  </si>
+  <si>
+    <t>id_obrasocial</t>
+  </si>
+  <si>
+    <t>dni</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>id_servicio</t>
+  </si>
+  <si>
+    <t>id_medico</t>
+  </si>
+  <si>
+    <t>atencion</t>
+  </si>
+  <si>
+    <t>Obra Social</t>
+  </si>
+  <si>
+    <t>matricula</t>
+  </si>
+  <si>
+    <t>descuento</t>
+  </si>
+  <si>
+    <t>cuit</t>
+  </si>
+  <si>
+    <t>id_razon</t>
+  </si>
+  <si>
+    <t>Razon Social</t>
+  </si>
+  <si>
+    <t>legajo</t>
+  </si>
+  <si>
+    <t>e-mail</t>
+  </si>
+  <si>
+    <t>fecha_baja</t>
+  </si>
+  <si>
+    <t>caracteristica</t>
+  </si>
+  <si>
     <t>Caracteristicas</t>
-  </si>
-  <si>
-    <t>Tipos Productos</t>
-  </si>
-  <si>
-    <t>Tipos Caracteristicas</t>
-  </si>
-  <si>
-    <t>id_producto</t>
-  </si>
-  <si>
-    <t>id_t_caracteristica</t>
-  </si>
-  <si>
-    <t>id_caracteristica</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
-    <t>detalles</t>
-  </si>
-  <si>
-    <t>Sedes</t>
-  </si>
-  <si>
-    <t>Puestos</t>
-  </si>
-  <si>
-    <t>puesto</t>
-  </si>
-  <si>
-    <t>id_sede</t>
-  </si>
-  <si>
-    <t>calle</t>
-  </si>
-  <si>
-    <t>Proveedores</t>
-  </si>
-  <si>
-    <t>id_proveedor</t>
-  </si>
-  <si>
-    <t>Pedidos</t>
-  </si>
-  <si>
-    <t>id_pedido</t>
-  </si>
-  <si>
-    <t>Detalle Pedido</t>
-  </si>
-  <si>
-    <t>id_det_ped</t>
-  </si>
-  <si>
-    <t>stock</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>precio compra</t>
-  </si>
-  <si>
-    <t>id_puesto</t>
-  </si>
-  <si>
-    <t>Paises</t>
-  </si>
-  <si>
-    <t>Clientes</t>
-  </si>
-  <si>
-    <t>Productos</t>
-  </si>
-  <si>
-    <t>Medicos</t>
-  </si>
-  <si>
-    <t>Empleados</t>
-  </si>
-  <si>
-    <t>activo</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>sueldo</t>
-  </si>
-  <si>
-    <t>id_obrasocial</t>
-  </si>
-  <si>
-    <t>dni</t>
-  </si>
-  <si>
-    <t>sexo</t>
-  </si>
-  <si>
-    <t>Servicio</t>
-  </si>
-  <si>
-    <t>id_servicio</t>
-  </si>
-  <si>
-    <t>id_medico</t>
-  </si>
-  <si>
-    <t>atencion</t>
-  </si>
-  <si>
-    <t>Obra Social</t>
-  </si>
-  <si>
-    <t>matricula</t>
-  </si>
-  <si>
-    <t>descuento</t>
-  </si>
-  <si>
-    <t>cuit</t>
-  </si>
-  <si>
-    <t>id_razon</t>
-  </si>
-  <si>
-    <t>Razon Social</t>
-  </si>
-  <si>
-    <t>legajo</t>
-  </si>
-  <si>
-    <t>e-mail</t>
-  </si>
-  <si>
-    <t>fecha_baja</t>
   </si>
 </sst>
 </file>
@@ -714,15 +708,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -730,9 +724,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="3067050" y="3362325"/>
-          <a:ext cx="1247775" cy="581025"/>
+        <a:xfrm>
+          <a:off x="5953125" y="3600450"/>
+          <a:ext cx="723900" cy="314325"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -763,76 +757,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>816510</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95248</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>98279</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>200648</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>77590</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="82" name="Arco 81"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="21447408">
-          <a:off x="3102510" y="2384279"/>
-          <a:ext cx="650963" cy="1312811"/>
-        </a:xfrm>
-        <a:prstGeom prst="arc">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 16200000"/>
-            <a:gd name="adj2" fmla="val 5636372"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF5353"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-AR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>285746</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -841,8 +775,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="6457949" y="2390775"/>
-          <a:ext cx="504822" cy="1724025"/>
+          <a:off x="6457948" y="2390774"/>
+          <a:ext cx="571501" cy="1895475"/>
         </a:xfrm>
         <a:prstGeom prst="arc">
           <a:avLst>
@@ -2002,7 +1936,7 @@
   <dimension ref="B1:AR33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,10 +1991,10 @@
     </row>
     <row r="2" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C2" s="33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I2" s="23"/>
       <c r="P2" s="25"/>
@@ -2082,19 +2016,19 @@
         <v>35</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I3" s="23"/>
       <c r="K3" s="8" t="s">
@@ -2108,13 +2042,13 @@
         <v>19</v>
       </c>
       <c r="V3" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="Z3" s="9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AD3" s="27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AG3" s="26"/>
       <c r="AH3" s="30"/>
@@ -2134,13 +2068,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I4" s="23"/>
       <c r="J4" s="2" t="s">
@@ -2150,7 +2084,7 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>35</v>
@@ -2159,7 +2093,7 @@
         <v>16</v>
       </c>
       <c r="P4" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>35</v>
@@ -2168,16 +2102,16 @@
         <v>24</v>
       </c>
       <c r="T4" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="W4" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>35</v>
@@ -2186,16 +2120,16 @@
         <v>14</v>
       </c>
       <c r="AA4" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AC4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AD4" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AE4" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG4" s="26"/>
       <c r="AH4" s="30"/>
@@ -2215,16 +2149,16 @@
         <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="1" t="s">
@@ -2234,37 +2168,37 @@
         <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="W5" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Z5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AD5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="AE5" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG5" s="26"/>
       <c r="AH5" s="30"/>
@@ -2284,26 +2218,26 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I6" s="23"/>
       <c r="J6" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>36</v>
@@ -2312,19 +2246,19 @@
         <v>11</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="W6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AA6" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG6" s="26"/>
       <c r="AH6" s="30"/>
@@ -2341,29 +2275,29 @@
     </row>
     <row r="7" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>36</v>
@@ -2372,7 +2306,7 @@
         <v>14</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="S7" s="8" t="s">
         <v>21</v>
@@ -2381,19 +2315,19 @@
         <v>36</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="W7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AA7" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG7" s="26"/>
       <c r="AH7" s="30"/>
@@ -2410,23 +2344,23 @@
     </row>
     <row r="8" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I8" s="23"/>
       <c r="K8" s="17" t="s">
         <v>2</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>36</v>
@@ -2435,7 +2369,7 @@
         <v>24</v>
       </c>
       <c r="P8" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>35</v>
@@ -2444,16 +2378,16 @@
         <v>22</v>
       </c>
       <c r="T8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="W8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>36</v>
@@ -2462,7 +2396,7 @@
         <v>12</v>
       </c>
       <c r="AA8" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG8" s="26"/>
       <c r="AH8" s="30"/>
@@ -2479,50 +2413,50 @@
     </row>
     <row r="9" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>85</v>
-      </c>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I9" s="23"/>
       <c r="K9" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P9" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="T9" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="V9" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="W9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="AA9" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG9" s="26"/>
       <c r="AH9" s="30"/>
@@ -2545,20 +2479,20 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>36</v>
@@ -2567,19 +2501,19 @@
         <v>22</v>
       </c>
       <c r="P10" s="23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V10" s="17" t="s">
         <v>13</v>
       </c>
       <c r="W10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Z10" s="17" t="s">
         <v>15</v>
       </c>
       <c r="AA10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG10" s="26"/>
       <c r="AH10" s="26"/>
@@ -2599,22 +2533,22 @@
         <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="V11" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="W11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Z11" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AA11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG11" s="26"/>
       <c r="AH11" s="26"/>
@@ -2631,13 +2565,10 @@
     </row>
     <row r="12" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P12" s="25"/>
       <c r="R12" s="2" t="s">
@@ -2647,19 +2578,19 @@
         <v>34</v>
       </c>
       <c r="T12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V12" s="17" t="s">
         <v>15</v>
       </c>
       <c r="W12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="AA12" s="25" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AG12" s="26"/>
       <c r="AH12" s="26"/>
@@ -2679,24 +2610,15 @@
         <v>35</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H13" s="25"/>
-      <c r="J13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" t="s">
-        <v>57</v>
-      </c>
       <c r="N13" s="2" t="s">
         <v>35</v>
       </c>
@@ -2704,7 +2626,7 @@
         <v>6</v>
       </c>
       <c r="P13" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>36</v>
@@ -2713,13 +2635,13 @@
         <v>16</v>
       </c>
       <c r="T13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V13" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="W13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG13" s="26"/>
       <c r="AH13" s="26"/>
@@ -2739,43 +2661,37 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P14" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>36</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="T14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="W14" s="23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AG14" s="26"/>
       <c r="AH14" s="26"/>
@@ -2795,16 +2711,16 @@
         <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="O15" s="13"/>
       <c r="P15" s="25"/>
@@ -2812,7 +2728,7 @@
         <v>4</v>
       </c>
       <c r="T15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG15" s="26"/>
       <c r="AH15" s="26"/>
@@ -2835,17 +2751,17 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P16" s="25"/>
       <c r="S16" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T16" s="23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="V16" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Z16" s="10" t="s">
         <v>28</v>
@@ -2871,16 +2787,13 @@
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="24"/>
       <c r="H17" s="26"/>
-      <c r="K17" s="14" t="s">
-        <v>37</v>
-      </c>
       <c r="O17" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P17" s="25"/>
       <c r="R17" s="1"/>
@@ -2890,10 +2803,10 @@
         <v>35</v>
       </c>
       <c r="V17" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="W17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>35</v>
@@ -2902,10 +2815,10 @@
         <v>12</v>
       </c>
       <c r="AA17" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AD17" s="19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AG17" s="26"/>
       <c r="AH17" s="26"/>
@@ -2923,44 +2836,38 @@
     <row r="18" spans="2:44" x14ac:dyDescent="0.25">
       <c r="G18" s="23"/>
       <c r="H18" s="26"/>
-      <c r="J18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" t="s">
-        <v>57</v>
+      <c r="K18" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="W18" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AA18" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AC18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AD18" s="34" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AE18" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG18" s="26"/>
       <c r="AH18" s="26"/>
@@ -2978,17 +2885,20 @@
     <row r="19" spans="2:44" x14ac:dyDescent="0.25">
       <c r="G19" s="23"/>
       <c r="H19" s="26"/>
-      <c r="K19" s="3" t="s">
-        <v>44</v>
+      <c r="J19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="L19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="O19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Y19" s="1" t="s">
         <v>36</v>
@@ -2997,13 +2907,13 @@
         <v>26</v>
       </c>
       <c r="AA19" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AD19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="AE19" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG19" s="26"/>
       <c r="AH19" s="26"/>
@@ -3020,30 +2930,27 @@
     </row>
     <row r="20" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C20" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G20" s="23"/>
       <c r="H20" s="26"/>
-      <c r="J20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>41</v>
+      <c r="K20" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="L20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="P20" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AD20" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AE20" s="26" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG20" s="26"/>
       <c r="AH20" s="26"/>
@@ -3063,27 +2970,21 @@
         <v>35</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G21" s="23"/>
       <c r="H21" s="26"/>
-      <c r="J21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K21" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="L21" t="s">
-        <v>57</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>61</v>
+      <c r="O21" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="Z21" s="10" t="s">
         <v>27</v>
@@ -3092,7 +2993,7 @@
         <v>15</v>
       </c>
       <c r="AE21" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG21" s="26"/>
       <c r="AH21" s="26"/>
@@ -3112,19 +3013,16 @@
         <v>36</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="P22" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Y22" s="2" t="s">
         <v>35</v>
@@ -3133,13 +3031,13 @@
         <v>26</v>
       </c>
       <c r="AA22" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AD22" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AE22" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG22" s="26"/>
       <c r="AH22" s="26"/>
@@ -3159,25 +3057,25 @@
         <v>36</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Z23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="AA23" s="25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AC23" s="1" t="s">
         <v>36</v>
@@ -3186,7 +3084,7 @@
         <v>12</v>
       </c>
       <c r="AE23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG23" s="26"/>
       <c r="AH23" s="26"/>
@@ -3206,7 +3104,7 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>7</v>
@@ -3215,10 +3113,10 @@
         <v>36</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="P24" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>36</v>
@@ -3227,7 +3125,7 @@
         <v>31</v>
       </c>
       <c r="AA24" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG24" s="26"/>
       <c r="AH24" s="26"/>
@@ -3247,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>35</v>
@@ -3256,16 +3154,16 @@
         <v>8</v>
       </c>
       <c r="L25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O25" s="6" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="P25" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG25" s="26"/>
       <c r="AH25" s="26"/>
@@ -3285,16 +3183,19 @@
         <v>9</v>
       </c>
       <c r="L26" t="s">
-        <v>58</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="P26" s="26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Z26" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AG26" s="26"/>
       <c r="AH26" s="26"/>
@@ -3311,7 +3212,13 @@
     </row>
     <row r="27" spans="2:44" x14ac:dyDescent="0.25">
       <c r="C27" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="O27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="P27" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="Y27" s="2" t="s">
         <v>35</v>
@@ -3320,7 +3227,7 @@
         <v>31</v>
       </c>
       <c r="AA27" s="25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AG27" s="26"/>
       <c r="AH27" s="26"/>
@@ -3340,16 +3247,16 @@
         <v>35</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Z28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="AA28" s="25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG28" s="26"/>
       <c r="AH28" s="26"/>
@@ -3369,7 +3276,7 @@
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AG29" s="26"/>
       <c r="AH29" s="26"/>

</xml_diff>